<commit_message>
Repositories and Services Added
</commit_message>
<xml_diff>
--- a/Notes/eCommerceDatabase.xlsx
+++ b/Notes/eCommerceDatabase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuced\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuced\Desktop\e-Commerce\e-Commerce Back-End\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFFFCC0-0E56-42C1-8433-1477F809DFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223A0AF3-79B2-4792-924E-F2361EABBF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{B099DB66-700E-46C4-AFEC-10A86677196D}"/>
   </bookViews>
@@ -1074,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B851C4-08D6-4C48-8CB9-26DA5F5364D7}">
   <dimension ref="A1:U138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="E49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K61" sqref="K61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.84375" defaultRowHeight="23.6" customHeight="1" x14ac:dyDescent="0.4"/>

</xml_diff>